<commit_message>
update for adding the OCNet
</commit_message>
<xml_diff>
--- a/others/Experiment Result Collecting.xlsx
+++ b/others/Experiment Result Collecting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizhixuan/Documents/OneDrive - www.office2016.cc/语义分割/segmentation-paper-reading-notes/others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="102_{79BBAE74-8D80-6948-98E9-539AF6DD0874}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4958D13D-78F7-0541-8F9C-A72B39FC24C0}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="102_{79BBAE74-8D80-6948-98E9-539AF6DD0874}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{CFDA7C5C-212B-6E47-AC6C-977984B11543}"/>
   <bookViews>
-    <workbookView xWindow="33020" yWindow="80" windowWidth="28800" windowHeight="17540" xr2:uid="{63B4AE39-E76B-CB44-97BF-80BBBCE4952D}"/>
+    <workbookView xWindow="38180" yWindow="400" windowWidth="28800" windowHeight="17540" xr2:uid="{63B4AE39-E76B-CB44-97BF-80BBBCE4952D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>mIoU%</t>
   </si>
@@ -203,10 +203,6 @@
   </si>
   <si>
     <t>RefineNet (Res101) (Lin et al. 2017)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coarse</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -228,6 +224,22 @@
   </si>
   <si>
     <t>ExFuse ResNeXt131 (Zhang et al. 2018)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fine mIoU%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coarse mIoU%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCNet(Res101) (Yuan et al. 2018)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以后得分别验证一下这些方法是只用了fine或coarse还是都用了</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -315,7 +327,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -348,6 +360,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -675,25 +690,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046A11F8-E99A-4346-8F43-B4230CF89546}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="168" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="168" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.5" style="2" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="14.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="29" style="2" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" thickBot="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="G1" s="1"/>
@@ -838,11 +855,11 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="17" customHeight="1" thickBot="1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="10"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -853,17 +870,17 @@
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="16" thickTop="1">
+    <row r="17" spans="1:5" ht="16" thickTop="1">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -872,7 +889,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -880,8 +897,11 @@
         <v>73.599999999999994</v>
       </c>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -890,7 +910,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -899,7 +919,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -910,7 +930,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -921,7 +941,7 @@
         <v>81.2</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -930,7 +950,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
@@ -939,7 +959,7 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
@@ -948,7 +968,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
@@ -957,16 +977,16 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5">
         <v>80.900000000000006</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
@@ -975,26 +995,30 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" ht="16" thickBot="1">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="5">
+        <v>81.7</v>
+      </c>
+      <c r="C29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" ht="16" thickBot="1">
+      <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="6">
+      <c r="B30" s="4"/>
+      <c r="C30" s="6">
         <v>82.1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="32" customHeight="1">
-      <c r="A31" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+    <row r="32" spans="1:5" ht="32" customHeight="1">
+      <c r="A32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
@@ -1006,237 +1030,238 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:5" ht="16" thickBot="1">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="16" thickBot="1">
+      <c r="A36" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="16" thickBot="1">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="16" thickBot="1">
+      <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="16" thickTop="1">
-      <c r="A37" s="1" t="s">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="16" thickTop="1">
+      <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B38" s="1">
         <v>22.7</v>
-      </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="1">
-        <v>26.9</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" s="1">
-        <v>31.2</v>
+        <v>26.9</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B40" s="1">
-        <v>33.6</v>
+        <v>31.2</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B42" s="1">
         <v>35.700000000000003</v>
       </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" ht="16" thickBot="1">
-      <c r="A42" s="4" t="s">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" ht="16" thickBot="1">
+      <c r="A43" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B43" s="4">
         <v>39.700000000000003</v>
       </c>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:5" ht="16" thickBot="1">
-      <c r="A45" s="13" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" ht="16" thickBot="1">
+      <c r="A46" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="13"/>
-    </row>
-    <row r="46" spans="1:5" ht="16" thickBot="1">
-      <c r="A46" s="8" t="s">
+      <c r="B46" s="14"/>
+    </row>
+    <row r="47" spans="1:5" ht="16" thickBot="1">
+      <c r="A47" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16" thickTop="1">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:5" ht="16" thickTop="1">
+      <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B48" s="1">
         <v>82.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="1">
-        <v>83.1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1">
-        <v>83.6</v>
+        <v>83.1</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B50" s="1">
-        <v>84.2</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B51" s="1">
-        <v>84.9</v>
+        <v>84.2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="1">
+        <v>84.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B53" s="1">
         <v>85.4</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="12">
+    <row r="54" spans="1:2">
+      <c r="A54" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="12">
         <v>86.2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B54" s="1">
-        <v>86.3</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B55" s="1">
-        <v>86.6</v>
+        <v>86.3</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" s="1">
-        <v>86.8</v>
+        <v>86.6</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B57" s="1">
-        <v>85.7</v>
+        <v>86.8</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B58" s="1">
-        <v>86.9</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="1">
+        <v>86.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B60" s="1">
         <v>87.8</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" s="12">
+    <row r="61" spans="1:2">
+      <c r="A61" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="12">
         <v>87.9</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16" thickBot="1">
-      <c r="A61" s="4" t="s">
+    <row r="62" spans="1:2" ht="16" thickBot="1">
+      <c r="A62" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B62" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16" thickBot="1">
-      <c r="A64" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B64" s="13"/>
-    </row>
     <row r="65" spans="1:2" ht="16" thickBot="1">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="14"/>
+    </row>
+    <row r="66" spans="1:2" ht="16" thickBot="1">
+      <c r="A66" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16" thickTop="1">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-    </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" ht="16" thickTop="1">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
     </row>
@@ -1280,17 +1305,21 @@
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
     </row>
-    <row r="78" spans="1:2" ht="16" thickBot="1">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
+    <row r="78" spans="1:2">
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
+    </row>
+    <row r="79" spans="1:2" ht="16" thickBot="1">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A15:C15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update for adding AAF
</commit_message>
<xml_diff>
--- a/others/Experiment Result Collecting.xlsx
+++ b/others/Experiment Result Collecting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizhixuan/Documents/OneDrive - www.office2016.cc/语义分割/segmentation-paper-reading-notes/others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="102_{79BBAE74-8D80-6948-98E9-539AF6DD0874}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D8350EB2-7ECA-B947-9CE7-E04E20452312}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="102_{79BBAE74-8D80-6948-98E9-539AF6DD0874}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{ED6B4D3F-2042-BA47-9714-299DD1B10E14}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-900" windowWidth="38400" windowHeight="21140" xr2:uid="{63B4AE39-E76B-CB44-97BF-80BBBCE4952D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>mIoU%</t>
   </si>
@@ -282,6 +282,10 @@
   </si>
   <si>
     <t xml:space="preserve">CCNet (Huang et al. 2018) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AAF (Ke et al. 2018)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -384,7 +388,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -437,6 +441,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -753,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046A11F8-E99A-4346-8F43-B4230CF89546}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1286,144 +1293,148 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="16" thickTop="1">
-      <c r="A50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="1">
-        <v>82.7</v>
+      <c r="A50" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="18">
+        <v>82.17</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B51" s="1">
-        <v>83.1</v>
+        <v>82.7</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" s="1">
-        <v>83.6</v>
+        <v>83.1</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B53" s="1">
-        <v>84.2</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B54" s="1">
-        <v>84.9</v>
+        <v>84.2</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="1">
+        <v>84.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B56" s="1">
         <v>85.4</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B57" s="9">
         <v>86.2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" s="1">
-        <v>86.3</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B58" s="1">
-        <v>86.6</v>
+        <v>86.3</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B59" s="1">
-        <v>86.8</v>
+        <v>86.6</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B60" s="1">
-        <v>85.7</v>
+        <v>86.8</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B61" s="1">
-        <v>86.9</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="1">
+        <v>86.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B63" s="1">
         <v>87.8</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="9" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B64" s="9">
         <v>87.9</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16" thickBot="1">
-      <c r="A64" s="4" t="s">
+    <row r="65" spans="1:2" ht="16" thickBot="1">
+      <c r="A65" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B65" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16" thickBot="1">
-      <c r="A67" s="15" t="s">
+    <row r="68" spans="1:2" ht="16" thickBot="1">
+      <c r="A68" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="15"/>
-    </row>
-    <row r="68" spans="1:2" ht="16" thickBot="1">
-      <c r="A68" s="6" t="s">
+      <c r="B68" s="15"/>
+    </row>
+    <row r="69" spans="1:2" ht="16" thickBot="1">
+      <c r="A69" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16" thickTop="1">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-    </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" ht="16" thickTop="1">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
     </row>
@@ -1467,13 +1478,17 @@
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
     </row>
-    <row r="81" spans="1:2" ht="16" thickBot="1">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
+    <row r="81" spans="1:2">
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+    </row>
+    <row r="82" spans="1:2" ht="16" thickBot="1">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A48:B48"/>

</xml_diff>